<commit_message>
sea sky round 1
</commit_message>
<xml_diff>
--- a/2022_results.xlsx
+++ b/2022_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/Uni_Work/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="201" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{238BD669-D6E4-4BC0-8B32-85D291221BD5}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{395919BB-AD48-4045-8568-C46B6773B834}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="30525" yWindow="1890" windowWidth="18075" windowHeight="15015" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
   <si>
     <t>Tricksy Taxonomy</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Leaf Slug</t>
+  </si>
+  <si>
+    <t>Eclectus Parrot</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA7A126-1676-F548-AFF2-D58DA2E40C88}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -693,7 +696,7 @@
         <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="P2" t="s">
         <v>46</v>
@@ -736,7 +739,7 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="P4" t="s">
         <v>48</v>
@@ -776,7 +779,7 @@
         <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P6" t="s">
         <v>50</v>
@@ -817,7 +820,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="O8" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="P8" t="s">
         <v>52</v>
@@ -857,7 +860,7 @@
         <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="P10" t="s">
         <v>54</v>
@@ -897,7 +900,7 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="P12" t="s">
         <v>55</v>
@@ -937,7 +940,7 @@
         <v>30</v>
       </c>
       <c r="O14" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="P14" t="s">
         <v>56</v>
@@ -977,7 +980,7 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="P16" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
why not both round 1
</commit_message>
<xml_diff>
--- a/2022_results.xlsx
+++ b/2022_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/Uni_Work/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{395919BB-AD48-4045-8568-C46B6773B834}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41776BB9-034E-4640-92E2-E836E118FA6D}"/>
   <bookViews>
-    <workbookView xWindow="30525" yWindow="1890" windowWidth="18075" windowHeight="15015" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA7A126-1676-F548-AFF2-D58DA2E40C88}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1040,7 +1040,7 @@
         <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="P19" t="s">
         <v>58</v>
@@ -1083,7 +1083,7 @@
         <v>30</v>
       </c>
       <c r="O21" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="P21" t="s">
         <v>65</v>
@@ -1123,7 +1123,7 @@
         <v>30</v>
       </c>
       <c r="O23" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="P23" t="s">
         <v>66</v>
@@ -1163,7 +1163,7 @@
         <v>30</v>
       </c>
       <c r="O25" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="P25" t="s">
         <v>67</v>
@@ -1203,7 +1203,7 @@
         <v>30</v>
       </c>
       <c r="O27" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="P27" t="s">
         <v>69</v>
@@ -1243,7 +1243,7 @@
         <v>30</v>
       </c>
       <c r="O29" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="P29" t="s">
         <v>73</v>
@@ -1283,7 +1283,7 @@
         <v>30</v>
       </c>
       <c r="O31" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="P31" t="s">
         <v>75</v>
@@ -1323,7 +1323,7 @@
         <v>30</v>
       </c>
       <c r="O33" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="P33" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
temporary fix of broken brackets
</commit_message>
<xml_diff>
--- a/2022_results.xlsx
+++ b/2022_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/Uni_Work/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41776BB9-034E-4640-92E2-E836E118FA6D}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84167A94-C528-45A5-A2E9-9D89EC288F3C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA7A126-1676-F548-AFF2-D58DA2E40C88}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -693,7 +693,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="O2" t="s">
         <v>46</v>
@@ -736,7 +736,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="O4" t="s">
         <v>48</v>
@@ -776,7 +776,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O6" t="s">
         <v>50</v>
@@ -816,7 +816,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1"/>
       <c r="O8" t="s">
@@ -857,7 +857,7 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="O10" t="s">
         <v>79</v>
@@ -897,7 +897,7 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O12" t="s">
         <v>55</v>
@@ -937,7 +937,7 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O14" t="s">
         <v>62</v>
@@ -977,7 +977,7 @@
         <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O16" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
round 2 sea sky double
</commit_message>
<xml_diff>
--- a/2022_results.xlsx
+++ b/2022_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/Uni_Work/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C09A4F5B-62A1-4608-BD2B-A6998D8EEC77}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE15D6A5-49EF-415A-A444-AABD00D7276A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA7A126-1676-F548-AFF2-D58DA2E40C88}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -719,7 +719,7 @@
         <v>30</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="P3" t="s">
         <v>47</v>
@@ -799,7 +799,7 @@
         <v>30</v>
       </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="P7" t="s">
         <v>51</v>
@@ -880,7 +880,7 @@
         <v>30</v>
       </c>
       <c r="N11" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="P11" t="s">
         <v>60</v>
@@ -960,7 +960,7 @@
         <v>30</v>
       </c>
       <c r="N15" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="P15" t="s">
         <v>62</v>
@@ -1063,7 +1063,7 @@
         <v>30</v>
       </c>
       <c r="N20" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="P20" t="s">
         <v>64</v>
@@ -1143,7 +1143,7 @@
         <v>30</v>
       </c>
       <c r="N24" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="P24" t="s">
         <v>71</v>
@@ -1223,7 +1223,7 @@
         <v>30</v>
       </c>
       <c r="N28" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="P28" t="s">
         <v>72</v>
@@ -1303,7 +1303,7 @@
         <v>30</v>
       </c>
       <c r="N32" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="P32" t="s">
         <v>76</v>

</xml_diff>